<commit_message>
Scaled up optimisation (45 WTP, 2500 DMZ)
</commit_message>
<xml_diff>
--- a/Optimisation/dataset/fixed_cost.xlsx
+++ b/Optimisation/dataset/fixed_cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/daniel_tan3_sg_ey_com/Documents/Documents/GitHub/WalmartSales/Optimisation/dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/GitHub/WalmartSales/Optimisation/dataset2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_389E4624409F75591BF2496421B923068DCC48F6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{625E0AC6-D9FA-4F34-99AF-7A750E5A67B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD27D29-FCC5-A743-A912-FEC80BA5F079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35895" yWindow="4245" windowWidth="17235" windowHeight="9645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5720" yWindow="760" windowWidth="24520" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Low</t>
   </si>
@@ -55,13 +55,133 @@
   </si>
   <si>
     <t>Sungai Tengi</t>
+  </si>
+  <si>
+    <t>WTP1</t>
+  </si>
+  <si>
+    <t>WTP2</t>
+  </si>
+  <si>
+    <t>WTP3</t>
+  </si>
+  <si>
+    <t>WTP4</t>
+  </si>
+  <si>
+    <t>WTP5</t>
+  </si>
+  <si>
+    <t>WTP6</t>
+  </si>
+  <si>
+    <t>WTP7</t>
+  </si>
+  <si>
+    <t>WTP8</t>
+  </si>
+  <si>
+    <t>WTP9</t>
+  </si>
+  <si>
+    <t>WTP10</t>
+  </si>
+  <si>
+    <t>WTP11</t>
+  </si>
+  <si>
+    <t>WTP12</t>
+  </si>
+  <si>
+    <t>WTP13</t>
+  </si>
+  <si>
+    <t>WTP14</t>
+  </si>
+  <si>
+    <t>WTP15</t>
+  </si>
+  <si>
+    <t>WTP16</t>
+  </si>
+  <si>
+    <t>WTP17</t>
+  </si>
+  <si>
+    <t>WTP18</t>
+  </si>
+  <si>
+    <t>WTP19</t>
+  </si>
+  <si>
+    <t>WTP20</t>
+  </si>
+  <si>
+    <t>WTP21</t>
+  </si>
+  <si>
+    <t>WTP22</t>
+  </si>
+  <si>
+    <t>WTP23</t>
+  </si>
+  <si>
+    <t>WTP24</t>
+  </si>
+  <si>
+    <t>WTP25</t>
+  </si>
+  <si>
+    <t>WTP26</t>
+  </si>
+  <si>
+    <t>WTP27</t>
+  </si>
+  <si>
+    <t>WTP28</t>
+  </si>
+  <si>
+    <t>WTP29</t>
+  </si>
+  <si>
+    <t>WTP30</t>
+  </si>
+  <si>
+    <t>WTP31</t>
+  </si>
+  <si>
+    <t>WTP32</t>
+  </si>
+  <si>
+    <t>WTP33</t>
+  </si>
+  <si>
+    <t>WTP34</t>
+  </si>
+  <si>
+    <t>WTP35</t>
+  </si>
+  <si>
+    <t>WTP36</t>
+  </si>
+  <si>
+    <t>WTP37</t>
+  </si>
+  <si>
+    <t>WTP38</t>
+  </si>
+  <si>
+    <t>WTP39</t>
+  </si>
+  <si>
+    <t>WTP40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +194,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -430,20 +556,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -454,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -465,7 +591,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -476,7 +602,7 @@
         <v>7270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -487,30 +613,311 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B45" s="3">
         <v>3230</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C45" s="3">
         <v>4730</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B46" s="3">
         <v>2110</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C46" s="3">
         <f>3080*2</f>
         <v>6160</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>